<commit_message>
started unit economics build, added folders for OEM ER
</commit_message>
<xml_diff>
--- a/ISSC/4. Model/ISSC_Valuation_Model_20240522_v1.xlsx
+++ b/ISSC/4. Model/ISSC_Valuation_Model_20240522_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndrewChen\Downloads\ISSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Desktop\ER\ISSC\4. Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3CCE39-27CC-4B53-A084-13BA4C6DE1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A32A26-563B-4C05-819D-B07CC6CE4C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{81AE2BAB-5DCF-4ACF-AB76-A5C9ECDD0E8C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81AE2BAB-5DCF-4ACF-AB76-A5C9ECDD0E8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Earnings Model" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Product</t>
   </si>
@@ -192,9 +192,6 @@
     <t>EPS:</t>
   </si>
   <si>
-    <t>Drivers</t>
-  </si>
-  <si>
     <t>(+) Interest</t>
   </si>
   <si>
@@ -208,6 +205,57 @@
   </si>
   <si>
     <t>EBITDA margin %</t>
+  </si>
+  <si>
+    <t>OEM CapEx</t>
+  </si>
+  <si>
+    <t>Unit Economics</t>
+  </si>
+  <si>
+    <t>Pilatus CapEx</t>
+  </si>
+  <si>
+    <t>Textron CapEx</t>
+  </si>
+  <si>
+    <t>Challenge Airlines CapEx</t>
+  </si>
+  <si>
+    <t>Air Transport Services Group CapEx</t>
+  </si>
+  <si>
+    <t>% of net sales</t>
+  </si>
+  <si>
+    <t>ISSC - Pilatus Revenue</t>
+  </si>
+  <si>
+    <t>ISSC - Textron Revenue</t>
+  </si>
+  <si>
+    <t>ISSC - Challenge Airlines Revenue</t>
+  </si>
+  <si>
+    <t>ISSC - ATSG Revenue</t>
+  </si>
+  <si>
+    <t>ISSC - Cargojet Inc. Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">think the build would be </t>
+  </si>
+  <si>
+    <t>OEM Aviation related rev -&gt; % CapEx of revenue -&gt; ISSC % of CapEx = ISSC XOEM revenue</t>
+  </si>
+  <si>
+    <t>OEM backlog -&gt; project OEM revenues (Backlog + % of new orders, perhaps use TAM CAGR) -&gt; % CapEx should be relatively stable going forward</t>
+  </si>
+  <si>
+    <t>Regress to find corr</t>
+  </si>
+  <si>
+    <t>project for each, then sum and subdivide between EDCs/service/product</t>
   </si>
 </sst>
 </file>
@@ -323,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -366,6 +414,10 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,47 +770,47 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:BJ63"/>
+  <dimension ref="B2:BJ80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="12" topLeftCell="O13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="E67" sqref="E67"/>
+      <selection pane="bottomRight" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="25" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.6640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.6640625" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.6640625" style="1"/>
+    <col min="1" max="1" width="9.7109375" style="1"/>
+    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
+    <col min="3" max="25" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.7109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.7109375" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:62" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:62" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:62" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:62" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>45434</v>
       </c>
     </row>
-    <row r="7" spans="2:62" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
@@ -823,7 +875,7 @@
       <c r="BI7" s="3"/>
       <c r="BJ7" s="3"/>
     </row>
-    <row r="9" spans="2:62" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1067,7 +1119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:62" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1308,7 +1360,7 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="11" spans="2:62" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:62" x14ac:dyDescent="0.25">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1370,7 +1422,7 @@
       <c r="BI11" s="6"/>
       <c r="BJ11" s="6"/>
     </row>
-    <row r="12" spans="2:62" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:62" x14ac:dyDescent="0.25">
       <c r="C12" s="13">
         <v>43100</v>
       </c>
@@ -1611,12 +1663,12 @@
         <v>48487</v>
       </c>
     </row>
-    <row r="14" spans="2:62" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:62" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1721,7 +1773,7 @@
         <v>4895.5889999999999</v>
       </c>
     </row>
-    <row r="16" spans="2:62" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
@@ -1810,7 +1862,7 @@
         <v>5098.2219999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
@@ -1897,7 +1949,7 @@
         <v>745.70500000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>3</v>
       </c>
@@ -2142,7 +2194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:62" x14ac:dyDescent="0.25">
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -2170,7 +2222,7 @@
       <c r="AA19" s="8"/>
       <c r="AB19" s="8"/>
     </row>
-    <row r="20" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
@@ -2201,8 +2253,7 @@
       <c r="AA20" s="8"/>
       <c r="AB20" s="8"/>
     </row>
-    <row r="21" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+    <row r="21" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>0</v>
       </c>
@@ -2307,8 +2358,7 @@
         <v>2347.6950000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+    <row r="22" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>1</v>
       </c>
@@ -2397,8 +2447,7 @@
         <v>2462.2600000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
+    <row r="23" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
@@ -2486,8 +2535,7 @@
         <v>347.19900000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
+    <row r="24" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>12</v>
       </c>
@@ -2732,7 +2780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:62" x14ac:dyDescent="0.25">
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -2760,7 +2808,7 @@
       <c r="AA25" s="8"/>
       <c r="AB25" s="8"/>
     </row>
-    <row r="26" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>13</v>
       </c>
@@ -3005,7 +3053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
         <v>14</v>
       </c>
@@ -3250,7 +3298,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>15</v>
       </c>
@@ -3495,7 +3543,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -3740,7 +3788,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
         <v>17</v>
       </c>
@@ -3985,13 +4033,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
+    <row r="33" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>19</v>
       </c>
@@ -4074,8 +4121,7 @@
         <v>1031.1189999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
+    <row r="34" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>20</v>
       </c>
@@ -4158,8 +4204,7 @@
         <v>2908.1930000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
+    <row r="35" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>21</v>
       </c>
@@ -4404,7 +4449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B37" s="12" t="s">
         <v>22</v>
       </c>
@@ -4649,7 +4694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
         <v>23</v>
       </c>
@@ -4894,8 +4939,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
+    <row r="40" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>24</v>
       </c>
@@ -4978,8 +5022,7 @@
         <v>-171.47</v>
       </c>
     </row>
-    <row r="41" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
+    <row r="41" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>25</v>
       </c>
@@ -5062,8 +5105,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
+    <row r="42" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>26</v>
       </c>
@@ -5146,8 +5188,7 @@
         <v>26.472000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
+    <row r="43" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>27</v>
       </c>
@@ -5392,8 +5433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
+    <row r="45" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>28</v>
       </c>
@@ -5477,8 +5517,7 @@
         <v>325.93599999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
+    <row r="46" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
         <v>29</v>
       </c>
@@ -5723,8 +5762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
+    <row r="47" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="22"/>
       <c r="C47" s="23"/>
       <c r="D47" s="23"/>
@@ -5787,10 +5825,9 @@
       <c r="BI47" s="23"/>
       <c r="BJ47" s="23"/>
     </row>
-    <row r="48" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
+    <row r="48" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C48" s="17">
         <f>C40-C41</f>
@@ -5897,10 +5934,9 @@
         <v>-207.67000000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
+    <row r="49" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C49" s="17">
         <f>C45</f>
@@ -6007,10 +6043,9 @@
         <v>325.93599999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
+    <row r="50" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C50" s="25">
         <v>103.36799999999999</v>
@@ -6111,10 +6146,9 @@
         <v>414.65600000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
+    <row r="51" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C51" s="18">
         <f>C46+SUM(C48:C50)</f>
@@ -6357,10 +6391,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
+    <row r="52" spans="2:62" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C52" s="11">
         <f>C51/C18</f>
@@ -6603,185 +6636,183 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:62" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
+    <row r="55" spans="2:62" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C55" s="21">
+      <c r="C55" s="29">
         <v>16783.129000000001</v>
       </c>
-      <c r="D55" s="21">
+      <c r="D55" s="29">
         <v>16800.243999999999</v>
       </c>
-      <c r="E55" s="21">
+      <c r="E55" s="29">
         <v>16816.838</v>
       </c>
-      <c r="F55" s="21">
+      <c r="F55" s="29">
         <v>16823.754000000001</v>
       </c>
-      <c r="G55" s="21">
+      <c r="G55" s="29">
         <v>16840.598999999998</v>
       </c>
-      <c r="H55" s="21">
+      <c r="H55" s="29">
         <v>16860.567999999999</v>
       </c>
-      <c r="I55" s="21">
+      <c r="I55" s="29">
         <v>16880.341</v>
       </c>
-      <c r="J55" s="21">
+      <c r="J55" s="29">
         <v>16888.691999999999</v>
       </c>
-      <c r="K55" s="21">
+      <c r="K55" s="29">
         <v>16909.036</v>
       </c>
-      <c r="L55" s="21">
+      <c r="L55" s="29">
         <v>16931.137999999999</v>
       </c>
-      <c r="M55" s="21">
+      <c r="M55" s="29">
         <v>16952.973000000002</v>
       </c>
-      <c r="N55" s="21">
+      <c r="N55" s="29">
         <v>16964.059000000001</v>
       </c>
-      <c r="O55" s="21">
+      <c r="O55" s="29">
         <v>17214.383999999998</v>
       </c>
-      <c r="P55" s="21">
+      <c r="P55" s="29">
         <v>17222.165000000001</v>
       </c>
-      <c r="Q55" s="21">
+      <c r="Q55" s="29">
         <v>17230.386999999999</v>
       </c>
-      <c r="R55" s="21">
+      <c r="R55" s="29">
         <v>17225.422999999999</v>
       </c>
-      <c r="S55" s="21">
+      <c r="S55" s="29">
         <v>17246.371999999999</v>
       </c>
-      <c r="T55" s="21">
+      <c r="T55" s="29">
         <v>17253.745999999999</v>
       </c>
-      <c r="U55" s="21">
+      <c r="U55" s="29">
         <v>17261.348999999998</v>
       </c>
-      <c r="V55" s="21">
+      <c r="V55" s="29">
         <v>17256.75</v>
       </c>
-      <c r="W55" s="21">
+      <c r="W55" s="29">
         <v>17316.766</v>
       </c>
-      <c r="X55" s="21">
+      <c r="X55" s="29">
         <v>17352.34</v>
       </c>
-      <c r="Y55" s="21">
+      <c r="Y55" s="29">
         <v>17576.969000000001</v>
       </c>
-      <c r="Z55" s="21">
+      <c r="Z55" s="29">
         <v>17400.659</v>
       </c>
-      <c r="AA55" s="21">
+      <c r="AA55" s="29">
         <v>17451.362000000001</v>
       </c>
-      <c r="AB55" s="21">
+      <c r="AB55" s="29">
         <v>17456.12</v>
       </c>
     </row>
-    <row r="56" spans="1:62" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
+    <row r="56" spans="2:62" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C56" s="21">
+      <c r="C56" s="29">
         <v>16783.129000000001</v>
       </c>
-      <c r="D56" s="21">
+      <c r="D56" s="29">
         <v>16800.243999999999</v>
       </c>
-      <c r="E56" s="21">
+      <c r="E56" s="29">
         <v>16816.838</v>
       </c>
-      <c r="F56" s="21">
+      <c r="F56" s="29">
         <v>16823.754000000001</v>
       </c>
-      <c r="G56" s="21">
+      <c r="G56" s="29">
         <v>16840.598999999998</v>
       </c>
-      <c r="H56" s="21">
+      <c r="H56" s="29">
         <v>16875.72</v>
       </c>
-      <c r="I56" s="21">
+      <c r="I56" s="29">
         <v>16978.643</v>
       </c>
-      <c r="J56" s="21">
+      <c r="J56" s="29">
         <v>17074.825000000001</v>
       </c>
-      <c r="K56" s="21">
+      <c r="K56" s="29">
         <v>17081.578000000001</v>
       </c>
-      <c r="L56" s="21">
+      <c r="L56" s="29">
         <v>17123.387999999999</v>
       </c>
-      <c r="M56" s="21">
+      <c r="M56" s="29">
         <v>17087.275000000001</v>
       </c>
-      <c r="N56" s="21">
+      <c r="N56" s="29">
         <v>17164.525000000001</v>
       </c>
-      <c r="O56" s="21">
+      <c r="O56" s="29">
         <v>17216.287</v>
       </c>
-      <c r="P56" s="21">
+      <c r="P56" s="29">
         <v>17223.998</v>
       </c>
-      <c r="Q56" s="21">
+      <c r="Q56" s="29">
         <v>17231.437999999998</v>
       </c>
-      <c r="R56" s="21">
+      <c r="R56" s="29">
         <v>17226.62</v>
       </c>
-      <c r="S56" s="21">
+      <c r="S56" s="29">
         <v>17246.371999999999</v>
       </c>
-      <c r="T56" s="21">
+      <c r="T56" s="29">
         <v>17253.745999999999</v>
       </c>
-      <c r="U56" s="21">
+      <c r="U56" s="29">
         <v>17265.797999999999</v>
       </c>
-      <c r="V56" s="21">
+      <c r="V56" s="29">
         <v>17257.870999999999</v>
       </c>
-      <c r="W56" s="21">
+      <c r="W56" s="29">
         <v>17326.177</v>
       </c>
-      <c r="X56" s="21">
+      <c r="X56" s="29">
         <v>17354.03</v>
       </c>
-      <c r="Y56" s="21">
+      <c r="Y56" s="29">
         <v>17577.588</v>
       </c>
-      <c r="Z56" s="21">
+      <c r="Z56" s="29">
         <v>17451.313999999998</v>
       </c>
-      <c r="AA56" s="21">
+      <c r="AA56" s="29">
         <v>17474.905999999999</v>
       </c>
-      <c r="AB56" s="21">
+      <c r="AB56" s="29">
         <v>17487.526999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B59" s="16" t="s">
         <v>31</v>
       </c>
@@ -7026,7 +7057,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="60" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B60" s="16" t="s">
         <v>32</v>
       </c>
@@ -7271,9 +7302,797 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="63" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="3"/>
+      <c r="T63" s="3"/>
+      <c r="U63" s="3"/>
+      <c r="V63" s="3"/>
+      <c r="W63" s="3"/>
+      <c r="X63" s="3"/>
+      <c r="Y63" s="3"/>
+      <c r="Z63" s="3"/>
+      <c r="AA63" s="3"/>
+      <c r="AB63" s="3"/>
+      <c r="AC63" s="3"/>
+      <c r="AD63" s="3"/>
+      <c r="AE63" s="3"/>
+      <c r="AF63" s="3"/>
+      <c r="AG63" s="3"/>
+      <c r="AH63" s="3"/>
+      <c r="AI63" s="3"/>
+      <c r="AJ63" s="3"/>
+      <c r="AK63" s="3"/>
+      <c r="AL63" s="3"/>
+      <c r="AM63" s="3"/>
+      <c r="AN63" s="3"/>
+      <c r="AO63" s="3"/>
+      <c r="AP63" s="3"/>
+      <c r="AQ63" s="3"/>
+      <c r="AR63" s="3"/>
+      <c r="AS63" s="3"/>
+      <c r="AT63" s="3"/>
+      <c r="AU63" s="3"/>
+      <c r="AV63" s="3"/>
+      <c r="AW63" s="3"/>
+      <c r="AX63" s="3"/>
+      <c r="AY63" s="3"/>
+      <c r="AZ63" s="3"/>
+      <c r="BA63" s="3"/>
+      <c r="BB63" s="3"/>
+      <c r="BC63" s="3"/>
+      <c r="BD63" s="3"/>
+      <c r="BE63" s="3"/>
+      <c r="BF63" s="3"/>
+      <c r="BG63" s="3"/>
+      <c r="BH63" s="3"/>
+      <c r="BI63" s="3"/>
+      <c r="BJ63" s="3"/>
+    </row>
+    <row r="64" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B64" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12"/>
+      <c r="P64" s="12"/>
+      <c r="Q64" s="12"/>
+      <c r="R64" s="12"/>
+      <c r="S64" s="12"/>
+      <c r="T64" s="12"/>
+      <c r="U64" s="12"/>
+      <c r="V64" s="12"/>
+      <c r="W64" s="12"/>
+      <c r="X64" s="12"/>
+      <c r="Y64" s="12"/>
+      <c r="Z64" s="12"/>
+      <c r="AA64" s="12"/>
+      <c r="AB64" s="12"/>
+      <c r="AC64" s="12"/>
+      <c r="AD64" s="12"/>
+      <c r="AE64" s="12"/>
+      <c r="AF64" s="12"/>
+      <c r="AG64" s="12"/>
+      <c r="AH64" s="12"/>
+      <c r="AI64" s="12"/>
+      <c r="AJ64" s="12"/>
+      <c r="AK64" s="12"/>
+      <c r="AL64" s="12"/>
+      <c r="AM64" s="12"/>
+      <c r="AN64" s="12"/>
+      <c r="AO64" s="12"/>
+      <c r="AP64" s="12"/>
+      <c r="AQ64" s="12"/>
+      <c r="AR64" s="12"/>
+      <c r="AS64" s="12"/>
+      <c r="AT64" s="12"/>
+      <c r="AU64" s="12"/>
+      <c r="AV64" s="12"/>
+      <c r="AW64" s="12"/>
+      <c r="AX64" s="12"/>
+      <c r="AY64" s="12"/>
+      <c r="AZ64" s="12"/>
+      <c r="BA64" s="12"/>
+      <c r="BB64" s="12"/>
+      <c r="BC64" s="12"/>
+      <c r="BD64" s="12"/>
+      <c r="BE64" s="12"/>
+      <c r="BF64" s="12"/>
+      <c r="BG64" s="12"/>
+      <c r="BH64" s="12"/>
+      <c r="BI64" s="12"/>
+      <c r="BJ64" s="12"/>
+    </row>
+    <row r="65" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X65" s="26"/>
+      <c r="AA65" s="26"/>
+      <c r="AB65" s="26"/>
+    </row>
+    <row r="66" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X66" s="26"/>
+      <c r="AB66" s="26"/>
+      <c r="AE66" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X67" s="26"/>
+      <c r="AA67" s="26"/>
+      <c r="AE67" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X68" s="26"/>
+      <c r="AE68" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AE69" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C71" s="8">
+        <f t="shared" ref="C71:AB71" si="176">C72*C18</f>
+        <v>0</v>
+      </c>
+      <c r="D71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="E71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="F71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="G71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="H71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="I71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="J71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="K71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="L71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="M71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="N71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="O71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="P71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="Q71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="R71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="S71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="T71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="U71" s="8">
+        <f t="shared" si="176"/>
+        <v>1872.71352</v>
+      </c>
+      <c r="V71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="W71" s="8">
+        <f t="shared" si="176"/>
+        <v>2476.1772800000003</v>
+      </c>
+      <c r="X71" s="8">
+        <f t="shared" si="176"/>
+        <v>1541.4953399999999</v>
+      </c>
+      <c r="Y71" s="8">
+        <f t="shared" si="176"/>
+        <v>1989.8019999999999</v>
+      </c>
+      <c r="Z71" s="8">
+        <f t="shared" si="176"/>
+        <v>0</v>
+      </c>
+      <c r="AA71" s="8">
+        <f t="shared" si="176"/>
+        <v>2699.3382699999997</v>
+      </c>
+      <c r="AB71" s="8">
+        <f t="shared" si="176"/>
+        <v>3007.06448</v>
+      </c>
+      <c r="AE71" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" spans="2:31" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="U72" s="28">
+        <v>0.27</v>
+      </c>
+      <c r="W72" s="28">
+        <v>0.38</v>
+      </c>
+      <c r="X72" s="28">
+        <v>0.21</v>
+      </c>
+      <c r="Y72" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="AA72" s="28">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AB72" s="28">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73" s="8">
+        <f t="shared" ref="C73:AB73" si="177">C74*C18</f>
+        <v>0</v>
+      </c>
+      <c r="D73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="E73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="F73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="G73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="H73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="I73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="J73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="K73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="L73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="M73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="N73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="O73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="P73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="Q73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="R73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="S73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="T73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="U73" s="8">
+        <f t="shared" si="177"/>
+        <v>1109.7561599999999</v>
+      </c>
+      <c r="V73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="W73" s="8">
+        <f t="shared" si="177"/>
+        <v>716.78816000000006</v>
+      </c>
+      <c r="X73" s="8">
+        <f t="shared" si="177"/>
+        <v>734.04539999999997</v>
+      </c>
+      <c r="Y73" s="8">
+        <f t="shared" si="177"/>
+        <v>795.92079999999999</v>
+      </c>
+      <c r="Z73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="AA73" s="8">
+        <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+      <c r="AB73" s="8">
+        <f t="shared" si="177"/>
+        <v>1825.7177200000001</v>
+      </c>
+    </row>
+    <row r="74" spans="2:31" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="U74" s="28">
+        <v>0.16</v>
+      </c>
+      <c r="W74" s="28">
+        <v>0.11</v>
+      </c>
+      <c r="X74" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="Y74" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="AB74" s="28">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="75" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C75" s="8">
+        <f t="shared" ref="C75:AB75" si="178">C76*C18</f>
+        <v>0</v>
+      </c>
+      <c r="D75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="E75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="F75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="G75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="H75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="I75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="J75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="K75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="L75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="M75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="N75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="O75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="P75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="Q75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="R75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="S75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="T75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="U75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="V75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="W75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="X75" s="8">
+        <f t="shared" si="178"/>
+        <v>1321.28172</v>
+      </c>
+      <c r="Y75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="Z75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="AA75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+      <c r="AB75" s="8">
+        <f t="shared" si="178"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:31" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="X76" s="28">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="77" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C77" s="8">
+        <f t="shared" ref="C77:AB77" si="179">C78*C18</f>
+        <v>0</v>
+      </c>
+      <c r="D77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="E77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="F77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="G77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="H77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="I77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="J77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="K77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="L77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="M77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="N77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="O77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="P77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="Q77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="R77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="S77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="T77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="U77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="V77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="W77" s="8">
+        <f t="shared" si="179"/>
+        <v>847.11328000000003</v>
+      </c>
+      <c r="X77" s="8">
+        <f t="shared" si="179"/>
+        <v>1174.47264</v>
+      </c>
+      <c r="Y77" s="8">
+        <f t="shared" si="179"/>
+        <v>1910.2099199999998</v>
+      </c>
+      <c r="Z77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="AA77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="AB77" s="8">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:31" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="W78" s="28">
+        <v>0.13</v>
+      </c>
+      <c r="X78" s="28">
+        <v>0.16</v>
+      </c>
+      <c r="Y78" s="28">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="79" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C79" s="8">
+        <f t="shared" ref="C79:AB79" si="180">C80*C18</f>
+        <v>0</v>
+      </c>
+      <c r="D79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="E79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="F79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="G79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="H79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="I79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="J79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="K79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="L79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="M79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="N79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="O79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="P79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="Q79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="R79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="S79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="T79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="U79" s="8">
+        <f t="shared" si="180"/>
+        <v>971.03664000000003</v>
+      </c>
+      <c r="V79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="W79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="X79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="Y79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="Z79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="AA79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="AB79" s="8">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:31" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="U80" s="28">
+        <v>0.14000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added key diligence questions, updated model
</commit_message>
<xml_diff>
--- a/ISSC/4. Model/ISSC_Valuation_Model_20240522_v1.xlsx
+++ b/ISSC/4. Model/ISSC_Valuation_Model_20240522_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Desktop\ER\ISSC\4. Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328E5903-6A71-4198-A2A1-88646BB884CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC64CA24-C7FC-4ED2-A167-D919733A3491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81AE2BAB-5DCF-4ACF-AB76-A5C9ECDD0E8C}"/>
   </bookViews>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
   <si>
     <t>Product</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>project for each, then sum and subdivide between EDCs/service/product</t>
+  </si>
+  <si>
+    <t>ISSC - Amazon Revenue</t>
   </si>
 </sst>
 </file>
@@ -774,13 +777,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="B2:BJ83"/>
+  <dimension ref="B2:BJ85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="N61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="12" topLeftCell="C63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="AB3" sqref="AB3"/>
+      <selection pane="bottomRight" activeCell="K69" sqref="K68:K69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7498,107 +7501,107 @@
         <v>46</v>
       </c>
       <c r="C74" s="8">
-        <f>C75*C18</f>
+        <f t="shared" ref="C74:AB74" si="176">C75*C18</f>
         <v>0</v>
       </c>
       <c r="D74" s="8">
-        <f>D75*D18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="E74" s="8">
-        <f>E75*E18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="F74" s="8">
-        <f>F75*F18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="G74" s="8">
-        <f>G75*G18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="H74" s="8">
-        <f>H75*H18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="I74" s="8">
-        <f>I75*I18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="J74" s="8">
-        <f>J75*J18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="K74" s="8">
-        <f>K75*K18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="L74" s="8">
-        <f>L75*L18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="M74" s="8">
-        <f>M75*M18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="N74" s="8">
-        <f>N75*N18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="O74" s="8">
-        <f>O75*O18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="P74" s="8">
-        <f>P75*P18</f>
-        <v>0</v>
+        <f t="shared" si="176"/>
+        <v>1280.4612500000001</v>
       </c>
       <c r="Q74" s="8">
-        <f>Q75*Q18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="R74" s="8">
-        <f>R75*R18</f>
+        <f t="shared" si="176"/>
         <v>0</v>
       </c>
       <c r="S74" s="8">
-        <f>S75*S18</f>
-        <v>0</v>
+        <f t="shared" si="176"/>
+        <v>1606.9867200000001</v>
       </c>
       <c r="T74" s="8">
-        <f>T75*T18</f>
-        <v>0</v>
+        <f t="shared" si="176"/>
+        <v>1985.2878000000001</v>
       </c>
       <c r="U74" s="8">
-        <f>U75*U18</f>
+        <f t="shared" si="176"/>
         <v>1872.71352</v>
       </c>
       <c r="V74" s="8">
-        <f>V75*V18</f>
-        <v>0</v>
+        <f>(0.22*(SUM(S18:V18))-SUM(S74:U74))</f>
+        <v>637.96486000000004</v>
       </c>
       <c r="W74" s="8">
-        <f>W75*W18</f>
+        <f t="shared" si="176"/>
         <v>2476.1772800000003</v>
       </c>
       <c r="X74" s="8">
-        <f>X75*X18</f>
+        <f t="shared" si="176"/>
         <v>1541.4953399999999</v>
       </c>
       <c r="Y74" s="8">
-        <f>Y75*Y18</f>
+        <f t="shared" si="176"/>
         <v>1989.8019999999999</v>
       </c>
       <c r="Z74" s="8">
-        <f>Z75*Z18</f>
-        <v>0</v>
+        <f>(0.23*SUM(W18:Z18))-SUM(W74:Y74)</f>
+        <v>1998.4833699999999</v>
       </c>
       <c r="AA74" s="8">
-        <f>AA75*AA18</f>
+        <f t="shared" si="176"/>
         <v>2699.3382699999997</v>
       </c>
       <c r="AB74" s="8">
-        <f>AB75*AB18</f>
+        <f t="shared" si="176"/>
         <v>3007.06448</v>
       </c>
       <c r="AE74" s="1" t="s">
@@ -7609,9 +7612,22 @@
       <c r="B75" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="P75" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="S75" s="28">
+        <v>0.24</v>
+      </c>
+      <c r="T75" s="28">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="U75" s="28">
         <v>0.27</v>
       </c>
+      <c r="V75" s="28">
+        <f>V74/V18</f>
+        <v>8.7836187776577035E-2</v>
+      </c>
       <c r="W75" s="28">
         <v>0.38</v>
       </c>
@@ -7620,6 +7636,10 @@
       </c>
       <c r="Y75" s="28">
         <v>0.25</v>
+      </c>
+      <c r="Z75" s="11">
+        <f>Z74/Z18</f>
+        <v>0.15381710659033088</v>
       </c>
       <c r="AA75" s="28">
         <v>0.28999999999999998</v>
@@ -7633,107 +7653,107 @@
         <v>47</v>
       </c>
       <c r="C76" s="8">
-        <f>C77*C18</f>
+        <f t="shared" ref="C76:AB76" si="177">C77*C18</f>
         <v>0</v>
       </c>
       <c r="D76" s="8">
-        <f>D77*D18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="E76" s="8">
-        <f>E77*E18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="F76" s="8">
-        <f>F77*F18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="G76" s="8">
-        <f>G77*G18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="H76" s="8">
-        <f>H77*H18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="I76" s="8">
-        <f>I77*I18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="J76" s="8">
-        <f>J77*J18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="K76" s="8">
-        <f>K77*K18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="L76" s="8">
-        <f>L77*L18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="M76" s="8">
-        <f>M77*M18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="N76" s="8">
-        <f>N77*N18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="O76" s="8">
-        <f>O77*O18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="P76" s="8">
-        <f>P77*P18</f>
-        <v>0</v>
+        <f t="shared" si="177"/>
+        <v>819.49520000000007</v>
       </c>
       <c r="Q76" s="8">
-        <f>Q77*Q18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="R76" s="8">
-        <f>R77*R18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="S76" s="8">
-        <f>S77*S18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="T76" s="8">
-        <f>T77*T18</f>
-        <v>0</v>
+        <f t="shared" si="177"/>
+        <v>684.58200000000011</v>
       </c>
       <c r="U76" s="8">
-        <f>U77*U18</f>
+        <f t="shared" si="177"/>
         <v>1109.7561599999999</v>
       </c>
       <c r="V76" s="8">
-        <f>V77*V18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="W76" s="8">
-        <f>W77*W18</f>
+        <f t="shared" si="177"/>
         <v>716.78816000000006</v>
       </c>
       <c r="X76" s="8">
-        <f>X77*X18</f>
+        <f t="shared" si="177"/>
         <v>734.04539999999997</v>
       </c>
       <c r="Y76" s="8">
-        <f>Y77*Y18</f>
+        <f t="shared" si="177"/>
         <v>795.92079999999999</v>
       </c>
       <c r="Z76" s="8">
-        <f>Z77*Z18</f>
-        <v>0</v>
+        <f>(0.1*SUM(W18:Z18))-SUM(W76:Y76)</f>
+        <v>1234.0969400000004</v>
       </c>
       <c r="AA76" s="8">
-        <f>AA77*AA18</f>
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
       <c r="AB76" s="8">
-        <f>AB77*AB18</f>
+        <f t="shared" si="177"/>
         <v>1825.7177200000001</v>
       </c>
     </row>
@@ -7741,9 +7761,16 @@
       <c r="B77" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="P77" s="28">
+        <v>0.16</v>
+      </c>
+      <c r="T77" s="28">
+        <v>0.1</v>
+      </c>
       <c r="U77" s="28">
         <v>0.16</v>
       </c>
+      <c r="V77" s="28"/>
       <c r="W77" s="28">
         <v>0.11</v>
       </c>
@@ -7752,6 +7779,10 @@
       </c>
       <c r="Y77" s="28">
         <v>0.1</v>
+      </c>
+      <c r="Z77" s="11">
+        <f>Z76/Z18</f>
+        <v>9.498463855757841E-2</v>
       </c>
       <c r="AB77" s="28">
         <v>0.17</v>
@@ -7762,107 +7793,107 @@
         <v>48</v>
       </c>
       <c r="C78" s="8">
-        <f>C79*C18</f>
+        <f t="shared" ref="C78:AB78" si="178">C79*C18</f>
         <v>0</v>
       </c>
       <c r="D78" s="8">
-        <f>D79*D18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="E78" s="8">
-        <f>E79*E18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="F78" s="8">
-        <f>F79*F18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="G78" s="8">
-        <f>G79*G18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="H78" s="8">
-        <f>H79*H18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="I78" s="8">
-        <f>I79*I18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="J78" s="8">
-        <f>J79*J18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="K78" s="8">
-        <f>K79*K18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="L78" s="8">
-        <f>L79*L18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="M78" s="8">
-        <f>M79*M18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="N78" s="8">
-        <f>N79*N18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="O78" s="8">
-        <f>O79*O18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="P78" s="8">
-        <f>P79*P18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="Q78" s="8">
-        <f>Q79*Q18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="R78" s="8">
-        <f>R79*R18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="S78" s="8">
-        <f>S79*S18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="T78" s="8">
-        <f>T79*T18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="U78" s="8">
-        <f>U79*U18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="V78" s="8">
-        <f>V79*V18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="W78" s="8">
-        <f>W79*W18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="X78" s="8">
-        <f>X79*X18</f>
+        <f t="shared" si="178"/>
         <v>1321.28172</v>
       </c>
       <c r="Y78" s="8">
-        <f>Y79*Y18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="Z78" s="8">
-        <f>Z79*Z18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="AA78" s="8">
-        <f>AA79*AA18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
       <c r="AB78" s="8">
-        <f>AB79*AB18</f>
+        <f t="shared" si="178"/>
         <v>0</v>
       </c>
     </row>
@@ -7879,107 +7910,107 @@
         <v>49</v>
       </c>
       <c r="C80" s="8">
-        <f>C81*C18</f>
+        <f t="shared" ref="C80:AB80" si="179">C81*C18</f>
         <v>0</v>
       </c>
       <c r="D80" s="8">
-        <f>D81*D18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="E80" s="8">
-        <f>E81*E18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="F80" s="8">
-        <f>F81*F18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="G80" s="8">
-        <f>G81*G18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="H80" s="8">
-        <f>H81*H18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="I80" s="8">
-        <f>I81*I18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="J80" s="8">
-        <f>J81*J18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="K80" s="8">
-        <f>K81*K18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="L80" s="8">
-        <f>L81*L18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="M80" s="8">
-        <f>M81*M18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="N80" s="8">
-        <f>N81*N18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="O80" s="8">
-        <f>O81*O18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="P80" s="8">
-        <f>P81*P18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="Q80" s="8">
-        <f>Q81*Q18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="R80" s="8">
-        <f>R81*R18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="S80" s="8">
-        <f>S81*S18</f>
-        <v>0</v>
+        <f t="shared" si="179"/>
+        <v>1673.9445000000001</v>
       </c>
       <c r="T80" s="8">
-        <f>T81*T18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="U80" s="8">
-        <f>U81*U18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="V80" s="8">
-        <f>V81*V18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="W80" s="8">
-        <f>W81*W18</f>
+        <f t="shared" si="179"/>
         <v>847.11328000000003</v>
       </c>
       <c r="X80" s="8">
-        <f>X81*X18</f>
+        <f t="shared" si="179"/>
         <v>1174.47264</v>
       </c>
       <c r="Y80" s="8">
-        <f>Y81*Y18</f>
+        <f t="shared" si="179"/>
         <v>1910.2099199999998</v>
       </c>
       <c r="Z80" s="8">
-        <f>Z81*Z18</f>
-        <v>0</v>
+        <f>(0.12*SUM(W18:Z18))-SUM(W80:Y80)</f>
+        <v>245.22572000000036</v>
       </c>
       <c r="AA80" s="8">
-        <f>AA81*AA18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
       <c r="AB80" s="8">
-        <f>AB81*AB18</f>
+        <f t="shared" si="179"/>
         <v>0</v>
       </c>
     </row>
@@ -7987,6 +8018,9 @@
       <c r="B81" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="S81" s="28">
+        <v>0.25</v>
+      </c>
       <c r="W81" s="28">
         <v>0.13</v>
       </c>
@@ -7995,6 +8029,10 @@
       </c>
       <c r="Y81" s="28">
         <v>0.24</v>
+      </c>
+      <c r="Z81" s="11">
+        <f>Z80/Z18</f>
+        <v>1.8874267996501114E-2</v>
       </c>
     </row>
     <row r="82" spans="2:28" x14ac:dyDescent="0.25">
@@ -8002,107 +8040,107 @@
         <v>50</v>
       </c>
       <c r="C82" s="8">
-        <f>C83*C18</f>
+        <f t="shared" ref="C82:AB82" si="180">C83*C18</f>
         <v>0</v>
       </c>
       <c r="D82" s="8">
-        <f>D83*D18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="E82" s="8">
-        <f>E83*E18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="F82" s="8">
-        <f>F83*F18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="G82" s="8">
-        <f>G83*G18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="H82" s="8">
-        <f>H83*H18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="I82" s="8">
-        <f>I83*I18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="J82" s="8">
-        <f>J83*J18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="K82" s="8">
-        <f>K83*K18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="L82" s="8">
-        <f>L83*L18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="M82" s="8">
-        <f>M83*M18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="N82" s="8">
-        <f>N83*N18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="O82" s="8">
-        <f>O83*O18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="P82" s="8">
-        <f>P83*P18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="Q82" s="8">
-        <f>Q83*Q18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="R82" s="8">
-        <f>R83*R18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="S82" s="8">
-        <f>S83*S18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="T82" s="8">
-        <f>T83*T18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="U82" s="8">
-        <f>U83*U18</f>
+        <f t="shared" si="180"/>
         <v>971.03664000000003</v>
       </c>
       <c r="V82" s="8">
-        <f>V83*V18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="W82" s="8">
-        <f>W83*W18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="X82" s="8">
-        <f>X83*X18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="Y82" s="8">
-        <f>Y83*Y18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="Z82" s="8">
-        <f>Z83*Z18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="AA82" s="8">
-        <f>AA83*AA18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
       <c r="AB82" s="8">
-        <f>AB83*AB18</f>
+        <f t="shared" si="180"/>
         <v>0</v>
       </c>
     </row>
@@ -8113,6 +8151,20 @@
       <c r="U83" s="28">
         <v>0.14000000000000001</v>
       </c>
+    </row>
+    <row r="84" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B84" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B85" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="T85" s="26">
+        <v>0.11</v>
+      </c>
+      <c r="V85" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>